<commit_message>
[O] SM- remade graph for sprint 1
</commit_message>
<xml_diff>
--- a/Rapport/STATS.xlsx
+++ b/Rapport/STATS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stéphane\Desktop\Université\Session 4\LOG2990\log2990\Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7901E10A-A341-40D2-842B-35ADF20EA072}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC1C188-7638-487C-9320-3A732CF3D328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="4" xr2:uid="{DCFB863E-4B04-489E-871B-09E19AE8AA4C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{DCFB863E-4B04-489E-871B-09E19AE8AA4C}"/>
   </bookViews>
   <sheets>
     <sheet name="SPRINT1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4740" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="677">
   <si>
     <t>SPRINT1</t>
   </si>
@@ -2016,6 +2016,60 @@
   </si>
   <si>
     <t>02:22:20</t>
+  </si>
+  <si>
+    <t>16-janv</t>
+  </si>
+  <si>
+    <t>18-janv</t>
+  </si>
+  <si>
+    <t>22-janv</t>
+  </si>
+  <si>
+    <t>23-janv</t>
+  </si>
+  <si>
+    <t>24-janv</t>
+  </si>
+  <si>
+    <t>25-janv</t>
+  </si>
+  <si>
+    <t>28-janv</t>
+  </si>
+  <si>
+    <t>29-janv</t>
+  </si>
+  <si>
+    <t>30-janv</t>
+  </si>
+  <si>
+    <t>01-févr</t>
+  </si>
+  <si>
+    <t>02-févr</t>
+  </si>
+  <si>
+    <t>05-févr</t>
+  </si>
+  <si>
+    <t>26-janv</t>
+  </si>
+  <si>
+    <t>31-janv</t>
+  </si>
+  <si>
+    <t>03-févr</t>
+  </si>
+  <si>
+    <t>04-févr</t>
+  </si>
+  <si>
+    <t>janv</t>
+  </si>
+  <si>
+    <t>févr</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2089,6 +2143,9 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2174,63 +2231,112 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>SPRINT1!$A$3:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>Debug</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Debug,Dev</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Debug,Dev,Meeting</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dev</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Dev,Tests</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Dev,Tests,QA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Meeting</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>QA</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Tests</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Tests,QA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>SPRINT1!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>18-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>22-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>24-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>25-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>26-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>28-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>29-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>30-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>31-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>02-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>03-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>04-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>05-févr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>févr</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$B$3:$B$14</c:f>
+              <c:f>SPRINT1!$B$3:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="1">
-                  <c:v>1.68</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.6599999999999984</c:v>
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>4.13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.05</c:v>
+                  <c:v>1.95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.049999999999997</c:v>
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.1099999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2266,56 +2372,90 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>SPRINT1!$A$3:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>Debug</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Debug,Dev</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Debug,Dev,Meeting</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dev</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Dev,Tests</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Dev,Tests,QA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Meeting</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>QA</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Tests</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Tests,QA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>SPRINT1!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>18-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>22-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>24-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>25-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>26-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>28-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>29-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>30-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>31-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>02-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>03-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>04-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>05-févr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>févr</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$C$3:$C$14</c:f>
+              <c:f>SPRINT1!$C$3:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.5999999999999996</c:v>
+                <c:ptCount val="16"/>
+                <c:pt idx="5">
+                  <c:v>1.42</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -2352,51 +2492,103 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>SPRINT1!$A$3:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>Debug</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Debug,Dev</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Debug,Dev,Meeting</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dev</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Dev,Tests</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Dev,Tests,QA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Meeting</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>QA</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Tests</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Tests,QA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>SPRINT1!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>18-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>22-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>24-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>25-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>26-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>28-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>29-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>30-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>31-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>02-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>03-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>04-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>05-févr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>févr</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$D$3:$D$14</c:f>
+              <c:f>SPRINT1!$D$3:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>31.069999999999993</c:v>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>2.2400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.91</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2432,62 +2624,105 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>SPRINT1!$A$3:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>Debug</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Debug,Dev</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Debug,Dev,Meeting</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dev</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Dev,Tests</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Dev,Tests,QA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Meeting</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>QA</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Tests</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Tests,QA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>SPRINT1!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>18-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>22-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>24-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>25-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>26-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>28-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>29-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>30-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>31-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>02-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>03-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>04-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>05-févr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>févr</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$E$3:$E$14</c:f>
+              <c:f>SPRINT1!$E$3:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>22.31</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="15">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2524,69 +2759,115 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>SPRINT1!$A$3:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="1">
-                  <c:v>Debug</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Debug,Dev</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Debug,Dev,Meeting</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Dev</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Dev,Tests</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Dev,Tests,QA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Meeting</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>QA</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Tests</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Tests,QA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>SPRINT1!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>18-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>22-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>24-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>25-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>26-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>28-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>29-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>30-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>31-janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>01-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>02-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>03-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>04-févr</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>05-févr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>janv</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>févr</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SPRINT1!$F$3:$F$14</c:f>
+              <c:f>SPRINT1!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.33999999999999997</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.37</c:v>
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.39</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.73</c:v>
+                  <c:v>6.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.5399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>7.3999999999999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20153,16 +20434,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>302079</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>545646</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25397,7 +25678,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68F4A296-A329-4B72-B62D-C55748913FB4}" name="PivotTable11" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:G14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A1:G21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -25414,7 +25695,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="12">
         <item x="3"/>
         <item x="2"/>
@@ -25431,7 +25712,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField numFmtId="166" showAll="0">
+    <pivotField axis="axisRow" numFmtId="166" showAll="0">
       <items count="369">
         <item x="0"/>
         <item x="1"/>
@@ -25811,7 +26092,7 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="15">
         <item sd="0" x="0"/>
         <item x="1"/>
@@ -25831,42 +26112,64 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
+  <rowFields count="2">
+    <field x="16"/>
+    <field x="8"/>
   </rowFields>
-  <rowItems count="12">
-    <i>
-      <x/>
-    </i>
+  <rowItems count="19">
     <i>
       <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
     </i>
     <i>
       <x v="2"/>
     </i>
-    <i>
-      <x v="3"/>
+    <i r="1">
+      <x v="32"/>
     </i>
-    <i>
-      <x v="4"/>
+    <i r="1">
+      <x v="33"/>
     </i>
-    <i>
-      <x v="5"/>
+    <i r="1">
+      <x v="34"/>
     </i>
-    <i>
-      <x v="6"/>
+    <i r="1">
+      <x v="35"/>
     </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
+    <i r="1">
+      <x v="36"/>
     </i>
     <i t="grand">
       <x/>
@@ -26934,19 +27237,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44459F10-5AE9-414A-9254-9E33BCDA1576}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -26981,208 +27283,377 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="13" t="s">
+        <v>675</v>
+      </c>
+      <c r="B3" s="2">
+        <v>16.979999999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5.42</v>
+      </c>
       <c r="D3" s="2">
-        <v>31.069999999999993</v>
+        <v>20.66</v>
       </c>
       <c r="E3" s="2">
-        <v>22.31</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>25.31</v>
+      </c>
+      <c r="F3" s="2">
+        <v>21.99</v>
+      </c>
       <c r="G3" s="2">
-        <v>53.379999999999995</v>
+        <v>90.36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.68</v>
-      </c>
+      <c r="A4" s="17" t="s">
+        <v>659</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
       <c r="F4" s="2">
-        <v>2.5</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="G4" s="2">
-        <v>4.18</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="2"/>
+      <c r="A5" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.5</v>
+      </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>2.2400000000000002</v>
+      </c>
       <c r="E5" s="2">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>3.8099999999999996</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.29</v>
+      </c>
       <c r="G5" s="2">
-        <v>12</v>
+        <v>11.84</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>147</v>
+      <c r="A6" s="17" t="s">
+        <v>661</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2">
-        <v>8</v>
-      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>6</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="2">
-        <v>9.6599999999999984</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
+      <c r="A7" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <v>3.87</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2">
-        <v>20.37</v>
+        <v>2.48</v>
       </c>
       <c r="G7" s="2">
-        <v>37.629999999999995</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>452</v>
+      <c r="A8" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2">
-        <v>23.39</v>
-      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <v>23.39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.45</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.42</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.5</v>
+      </c>
       <c r="F9" s="2">
-        <v>7.73</v>
+        <v>6.15</v>
       </c>
       <c r="G9" s="2">
-        <v>7.73</v>
+        <v>12.98</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>243</v>
+      <c r="A10" s="17" t="s">
+        <v>671</v>
       </c>
       <c r="B10" s="2">
-        <v>2.5</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <v>2.5</v>
+        <v>2.0699999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>35</v>
+      <c r="A11" s="17" t="s">
+        <v>665</v>
       </c>
       <c r="B11" s="2">
-        <v>5.05</v>
+        <v>4.13</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
-        <v>2</v>
-      </c>
+      <c r="D11" s="2">
+        <v>2.68</v>
+      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
       <c r="G11" s="2">
-        <v>7.25</v>
+        <v>7.28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>45</v>
+      <c r="A12" s="17" t="s">
+        <v>666</v>
       </c>
       <c r="B12" s="2">
-        <v>30.049999999999997</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>1.95</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>6.91</v>
+      </c>
       <c r="E12" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12" s="2">
-        <v>7.3999999999999995</v>
+        <v>3</v>
       </c>
       <c r="G12" s="2">
-        <v>47.449999999999996</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="17" t="s">
+        <v>667</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.59</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
       <c r="F13" s="2">
-        <v>0.74</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="G13" s="2">
-        <v>0.74</v>
+        <v>16.61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>1.74</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>676</v>
+      </c>
+      <c r="B15" s="2">
+        <v>31.96</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11.18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>10.41</v>
+      </c>
+      <c r="E15" s="2">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2">
+        <v>40.339999999999996</v>
+      </c>
+      <c r="G15" s="2">
+        <v>113.89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>668</v>
+      </c>
+      <c r="B16" s="2">
+        <v>10.48</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5.32</v>
+      </c>
+      <c r="E16" s="2">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9.56</v>
+      </c>
+      <c r="G16" s="2">
+        <v>41.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>669</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.18</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>12.84</v>
+      </c>
+      <c r="G17" s="2">
+        <v>29.919999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>673</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>674</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4.46</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="G19" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>670</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7.1099999999999994</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>6</v>
+      </c>
+      <c r="F20" s="2">
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="G20" s="2">
+        <v>25.599999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B21" s="2">
         <v>48.94</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C21" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="D14" s="2">
-        <v>31.069999999999993</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D21" s="2">
+        <v>31.07</v>
+      </c>
+      <c r="E21" s="2">
         <v>45.31</v>
       </c>
-      <c r="F14" s="2">
-        <v>62.330000000000013</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="F21" s="2">
+        <v>62.33</v>
+      </c>
+      <c r="G21" s="2">
         <v>204.24999999999997</v>
       </c>
     </row>
@@ -27196,7 +27667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348B73A5-60B7-4542-BAFD-BF88765B3D7D}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
@@ -49236,7 +49707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BEB81A-627B-4A62-BE17-552999A0FF22}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>

</xml_diff>